<commit_message>
upto CS4 report created
</commit_message>
<xml_diff>
--- a/lists/4-column/CS1.xlsx
+++ b/lists/4-column/CS1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t xml:space="preserve">Project #1</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">Average of closest 2 analogies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRWM</t>
   </si>
   <si>
     <t xml:space="preserve">Test Data Real Effort</t>
@@ -188,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L118"/>
+  <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A111" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D118" activeCellId="0" sqref="D118:E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4109,15 +4112,26 @@
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="1" t="n">
+        <f aca="false">(2*B112 + 1* B113) / 3</f>
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B119" s="4"/>
+      <c r="C119" s="1" t="n">
         <v>2855</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A110:B110"/>
     <mergeCell ref="A115:C115"/>
     <mergeCell ref="A117:B117"/>
     <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>